<commit_message>
Updated Tags & Expertise.
</commit_message>
<xml_diff>
--- a/Documents/Tags & Expertise.xlsx
+++ b/Documents/Tags & Expertise.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Tags &amp; Expertise" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>apache2</t>
   </si>
@@ -155,12 +156,6 @@
     <t>Mapping</t>
   </si>
   <si>
-    <t>msoffice</t>
-  </si>
-  <si>
-    <t>MS Office</t>
-  </si>
-  <si>
     <t>mssql</t>
   </si>
   <si>
@@ -176,12 +171,6 @@
     <t>My SQL</t>
   </si>
   <si>
-    <t>ontime</t>
-  </si>
-  <si>
-    <t>Axosoft OnTime</t>
-  </si>
-  <si>
     <t>openscad</t>
   </si>
   <si>
@@ -230,12 +219,6 @@
     <t>Silverlight</t>
   </si>
   <si>
-    <t>svg</t>
-  </si>
-  <si>
-    <t>SVG</t>
-  </si>
-  <si>
     <t>svn</t>
   </si>
   <si>
@@ -362,9 +345,6 @@
     <t>WebForms</t>
   </si>
   <si>
-    <t>OnTime</t>
-  </si>
-  <si>
     <t>Flash</t>
   </si>
   <si>
@@ -387,6 +367,30 @@
   </si>
   <si>
     <t>WinForms</t>
+  </si>
+  <si>
+    <t>winserver</t>
+  </si>
+  <si>
+    <t>Windows Server</t>
+  </si>
+  <si>
+    <t>ssrs</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server Reporting Services</t>
+  </si>
+  <si>
+    <t>highcharts</t>
+  </si>
+  <si>
+    <t>Highcharts</t>
+  </si>
+  <si>
+    <t>highmaps</t>
+  </si>
+  <si>
+    <t>Highmaps</t>
   </si>
 </sst>
 </file>
@@ -713,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,16 +733,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -770,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F52" si="0">"Tags.allTags.push(new Tag(""" &amp; A3 &amp; """, " &amp; IF(B3 = "", "null", """" &amp; B3 &amp; """") &amp; ", """ &amp; C3 &amp; """" &amp; IF(D3 = "", "",  ", " &amp; D3) &amp; "));"</f>
+        <f t="shared" ref="F3:F53" si="0">"Tags.allTags.push(new Tag(""" &amp; A3 &amp; """, " &amp; IF(B3 = "", "null", """" &amp; B3 &amp; """") &amp; ", """ &amp; C3 &amp; """" &amp; IF(D3 = "", "",  ", " &amp; D3) &amp; "));"</f>
         <v>Tags.allTags.push(new Tag("apache2", null, "Apache2", 6));</v>
       </c>
     </row>
@@ -821,13 +825,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -839,440 +843,434 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("ontime", "OnTime", "Axosoft OnTime", 7));</v>
+        <v>Tags.allTags.push(new Tag("bs", null, "Bootstrap", 8));</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("bs", null, "Bootstrap", 8));</v>
+        <v>Tags.allTags.push(new Tag("cs", null, "C#", 10));</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("cs", null, "C#", 10));</v>
+        <v>Tags.allTags.push(new Tag("cpp", null, "C++", 3));</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("cpp", null, "C++", 3));</v>
+        <v>Tags.allTags.push(new Tag("css", null, "CSS", 10));</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("css", null, "CSS", 10));</v>
+        <v>Tags.allTags.push(new Tag("css3", null, "CSS3", 10));</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("css3", null, "CSS3", 10));</v>
+        <v>Tags.allTags.push(new Tag("flash", null, "Flash", 3));</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("flash", null, "Flash", 3));</v>
+        <v>Tags.allTags.push(new Tag("git", null, "Git", 7));</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("git", null, "Git", 7));</v>
+        <v>Tags.allTags.push(new Tag("grails", null, "Grails", 3));</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("grails", null, "Grails", 3));</v>
+        <v>Tags.allTags.push(new Tag("highcharts", null, "Highcharts", 6));</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("html", null, "HTML", 10));</v>
+        <v>Tags.allTags.push(new Tag("highmaps", null, "Highmaps", 8));</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("html5", null, "HTML5", 10));</v>
+        <v>Tags.allTags.push(new Tag("html", null, "HTML", 10));</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="D19">
         <v>10</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("iis", "IIS", "Internet Information Services", 10));</v>
+        <v>Tags.allTags.push(new Tag("html5", null, "HTML5", 10));</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("java", null, "Java", 7));</v>
+        <v>Tags.allTags.push(new Tag("iis", "IIS", "Internet Information Services", 10));</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("js", "JS", "JavaScript", 10));</v>
+        <v>Tags.allTags.push(new Tag("java", null, "Java", 7));</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("ko", null, "Knockout", 7));</v>
+        <v>Tags.allTags.push(new Tag("js", "JS", "JavaScript", 10));</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("linux", null, "Linux", 6));</v>
+        <v>Tags.allTags.push(new Tag("ko", null, "Knockout", 7));</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>6</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("mantis", null, "Mantis", 6));</v>
+        <v>Tags.allTags.push(new Tag("linux", null, "Linux", 6));</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("mapping", null, "Mapping", 6));</v>
+        <v>Tags.allTags.push(new Tag("mantis", null, "Mantis", 8));</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("mssql", "MS SQL", "Microsoft SQL Server", 9));</v>
+        <v>Tags.allTags.push(new Tag("mapping", null, "Mapping", 6));</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("mvc", "MVC", "ASP.NET MVC", 10));</v>
+        <v>Tags.allTags.push(new Tag("mssql", "MS SQL", "Microsoft SQL Server", 9));</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("msoffice", null, "MS Office", 6));</v>
+        <f>"Tags.allTags.push(new Tag(""" &amp; A28 &amp; """, " &amp; IF(B28 = "", "null", """" &amp; B28 &amp; """") &amp; ", """ &amp; C28 &amp; """" &amp; IF(D28 = "", "",  ", " &amp; D28) &amp; "));"</f>
+        <v>Tags.allTags.push(new Tag("ssrs", null, "Microsoft SQL Server Reporting Services", 8));</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("mysql", null, "My SQL", 7));</v>
+        <v>Tags.allTags.push(new Tag("mvc", "MVC", "ASP.NET MVC", 10));</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("openscad", null, "OpenSCAD", 3));</v>
+        <v>Tags.allTags.push(new Tag("mysql", null, "My SQL", 8));</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("oracle", null, "Oracle", 5));</v>
+        <v>Tags.allTags.push(new Tag("openscad", null, "OpenSCAD", 3));</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D32">
         <v>5</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("php", null, "PHP", 5));</v>
+        <v>Tags.allTags.push(new Tag("oracle", null, "Oracle", 5));</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("python", null, "Python", 2));</v>
+        <v>Tags.allTags.push(new Tag("php", null, "PHP", 5));</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("redmine", null, "Redmine", 6));</v>
+        <v>Tags.allTags.push(new Tag("python", null, "Python", 2));</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D35">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("regex", "RegEx", "Regular Expressions", 9));</v>
+        <v>Tags.allTags.push(new Tag("redmine", null, "Redmine", 6));</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,94 +1278,97 @@
         <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
         <v>61</v>
       </c>
       <c r="D36">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("rails", "Rails", "Ruby on Rails", 6));</v>
+        <v>Tags.allTags.push(new Tag("regex", "RegEx", "Regular Expressions", 9));</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("sl", null, "Silverlight", 4));</v>
+        <v>Tags.allTags.push(new Tag("rails", "Rails", "Ruby on Rails", 6));</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D38">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("svn", "SVN", "Subversion", 9));</v>
+        <v>Tags.allTags.push(new Tag("sl", null, "Silverlight", 4));</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("svg", null, "SVG", 7));</v>
+        <v>Tags.allTags.push(new Tag("svn", "SVN", "Subversion", 9));</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D40">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("tfs", "TFS", "Team Foundation Server", 9));</v>
+        <v>Tags.allTags.push(new Tag("tfs", "TFS", "Team Foundation Server", 6));</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -1379,10 +1380,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D42">
         <v>7</v>
@@ -1394,10 +1395,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D43">
         <v>7</v>
@@ -1409,13 +1410,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D44">
         <v>8</v>
@@ -1427,10 +1428,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -1442,111 +1443,126 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D46">
         <v>10</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="0"/>
+        <f>"Tags.allTags.push(new Tag(""" &amp; A46 &amp; """, " &amp; IF(B46 = "", "null", """" &amp; B46 &amp; """") &amp; ", """ &amp; C46 &amp; """" &amp; IF(D46 = "", "",  ", " &amp; D46) &amp; "));"</f>
         <v>Tags.allTags.push(new Tag("windows", null, "Windows", 10));</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("wcf", "WCF", "Windows Communication Foundation", 7));</v>
+        <v>Tags.allTags.push(new Tag("winserver", null, "Windows Server", 9));</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("winforms", "WinForms", "Windows Forms", 10));</v>
+        <v>Tags.allTags.push(new Tag("wcf", "WCF", "Windows Communication Foundation", 7));</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
+        <v>113</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("wp", null, "Windows Phone", 4));</v>
+        <v>Tags.allTags.push(new Tag("winforms", "WinForms", "Windows Forms", 10));</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("xml", null, "XML", 10));</v>
+        <v>Tags.allTags.push(new Tag("wp", null, "Windows Phone", 4));</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D51">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>Tags.allTags.push(new Tag("xsd", null, "XSD", 7));</v>
+        <v>Tags.allTags.push(new Tag("xml", null, "XML", 10));</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>Tags.allTags.push(new Tag("xsd", null, "XSD", 8));</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53">
         <v>9</v>
       </c>
-      <c r="F52" t="str">
+      <c r="F53" t="str">
         <f t="shared" si="0"/>
         <v>Tags.allTags.push(new Tag("xslt", null, "XSLT", 9));</v>
       </c>

</xml_diff>